<commit_message>
Fix Design Fix DataBase
</commit_message>
<xml_diff>
--- a/Tyuiu.PolyantsevEI.Sprint7.Project.V14/Properties/DataBase.xlsx
+++ b/Tyuiu.PolyantsevEI.Sprint7.Project.V14/Properties/DataBase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\source\repos\Tyuiu.PolyantsevEI.Sprint7\Tyuiu.PolyantsevEI.Sprint7.Project.V14\Properties\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92FE58E-9CF7-4CD2-A369-02ADA5049E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298229B4-CF65-4CAD-8C5E-15D6745AA4B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BA7D37AC-2523-46FA-BBD4-A61892A597A7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="441">
   <si>
     <t>Номер маршрута</t>
   </si>
@@ -57,9 +57,6 @@
     <t>да</t>
   </si>
   <si>
-    <t>АО "ТПАТП №1" 625019, г.Тюмень, ул.Республики, д.206А, ИНН 7203193689</t>
-  </si>
-  <si>
     <t>1д</t>
   </si>
   <si>
@@ -69,9 +66,6 @@
     <t>а/п Рощино, Гостиница, Больничный комплекс, ул. Бакинских Комиссаров, Дом Обороны, ул. Белинского, ул. Клары Цеткин, Президентское кадетское училище, Ипподром, Налоговая инспекция, ЖДВ, сквер Семёна Пацко, ул. Смоленская, Цветной бульвар 1, Центральный рынок 1, Станкостроительный завод, Тюменский драматический театр, ул. Фабричная, Родильный дом №2, сквер Гимназистов, ул. Харьковская, Травматология, ул. Одесская, Областная ГИБДД, Барабинская, ул. Гилевская, ул. Элеваторная, ул. Губкина, Озеро Оброчное, Школа № 67, мкр. Тура, ул. Западносибирская, Детский сад №62, ул. Энтузиастов</t>
   </si>
   <si>
-    <t>49,59 (21,91)</t>
-  </si>
-  <si>
     <t>п.Док – ул. Таллинская</t>
   </si>
   <si>
@@ -81,9 +75,6 @@
     <t>ул. Таллинская, ст. Войновка, ул. Боровская, ТЭЦ 2, ул. Теплотехников, Восточный 3, Сквер Десантников, Поликлиника, ул. Моторостроителей, Театр Ангажемент, сквер Депутатов, мкр. Тюменский, ул. Евгения Богдановича, ул. Прокопия Артамонова, ул. Н. Семёнова, Ожогина, ул. Федюнинского 43, ул. Федюнинского, мкр. Южный, (ул. Панфиловцев, ул. Закалужская) Школа №69, м‑н Пышма, Гимназия №49, ул. Пархоменко, ул. Транспортная, ул. Магнитогорская, Администрация Тюменского района, Спортцентр Энерго, Универсальный рынок, Московский тракт, ул. Кремлёвская, д. Плеханова, Сельхозтехника, Школа №51, ТЭМЗ, ул. Авторемонтная, з‑д Аккумуляторный, ул. Бакинских Комиссаров, Дом Обороны, Аллея Молодоженов, ул. Льва Толстого, Вечерняя школа №2, Строительный институт ТИУ, Сквер Святителя Филофея, ул. Подгорная, ул. Коммунистическая, ул. Тюменская, ул. Курчатова, п.ДОК.</t>
   </si>
   <si>
-    <t>56.56 (52,98)</t>
-  </si>
-  <si>
     <t>Центральный рынок – п. ММС</t>
   </si>
   <si>
@@ -93,9 +84,6 @@
     <t xml:space="preserve">п. ММС, Школа №45, сквер Мелиораторов, ул. Буровиков, з‑д Керамзитовый, УМВД по г.Тюмени, проезд Юганский, Стоматологическая Поликлиника №1, ул. Сеченова, озеро Алебашево, Алебашевский базар, ул. Циолковского, ул. Даудельная, ул. Володарского, Сквер Немцова, Центральный рынок </t>
   </si>
   <si>
-    <t xml:space="preserve">ООО "Тюменьавтотранс", 625026, Тюменская обл., г. Тюмень, проезд Воронинские горки, 142 стр. 4, оф. 7, ИНН 7203372991 </t>
-  </si>
-  <si>
     <t>4д</t>
   </si>
   <si>
@@ -108,27 +96,18 @@
     <t>ул. Электросетей, п. ММС, Школа №45, сквер Мелиораторов, ул. Буровиков, з-д Керамзитовый, УМВД по г.Тюмени, проезд Юганский, Стоматологическая Поликлиника №1, ул. Сеченова, озеро Алебашево, Алебашевский базар, ул. Циолковского, ул. Даудельная, ул. Володарского, Сквер Немцова, Центральный рынок</t>
   </si>
   <si>
-    <t>ООО "Тюменьавтотранс", 625026, Тюменская обл., г. Тюмень,проезд Воронинские горки, 142 стр. 4, оф. 7, ИНН 7203372991</t>
-  </si>
-  <si>
     <t>д. Матмасы, Детский сад №149, ул. Тимофея Чаркова, с/о Трудовик, Колледж водного транспорта, Сквер Корабельный, ул. Верхнетарманская, п. Тарманы, ул. Игримская, ДК Торфяник, парк им. Гагарина, Озеро Круглое, ул. Разведчика Кузнецова, Мост Мельникайте, Студенческий городок, Областная больница №2, Тюменский индустриальный университет, ул. Рижская, Площадь Памяти, Кардиоцентр,ул. 30 лет Победы, ул. В. Гнаровской, Сквер Победы, ул. Депутатская, АЗС, ул. Революции, ул. Федюнинского, мкр. Южный</t>
   </si>
   <si>
     <t>мкр. Южный, Школа №69, Городская юношеская библиотека, ул. Пышминская, ул. Молодежная, ул. Демьяна Бедного, ул. Салехардская, Гимназия №83, ул. Депутатская, Сквер Победы, ул. Валерии Гнаровской, Кардиоцентр, ул. Рижская, Тюменский индустриальный университет, Областная больница №2, Студенческий городок, Мост Мельникайте,  ул. Разведчика Кузнецова, Озеро Круглое, ул. Малышева, ДК Торфяник, ул. Игримская, Тарманы, ул. Верхнетарманская, Сквер Корабельный, ул. Беляева, ул. Малиновского, Колледж водного транспорта, с/о Трудовик, ул. Тимофея Чаркова, Детский сад №149, д. Матмасы</t>
   </si>
   <si>
-    <t xml:space="preserve">ИП Шулепов Сергей Михайлович 625017, Тюменская обл., г.Тюмень, ул. Черепанова, 76 ст. 6  ИНН 720400468814 </t>
-  </si>
-  <si>
     <t>ЖК Апрель, Детский сад №42, ул. Революции, ул. Депутатская, Сквер Победы, ул. Валерии Гнаровской, Площадь Памяти, ул. Таймырская, ул. Малыгина, ул. Шиллера, ул. Герцена, Цветной бульвар, ул. Первомайская, ул. Дзержинского, ул. 2-я Луговая, ул. Мысовская, ул. Астраханская, I Заречный микрорайон, II Заречный микрорайон, Автоколонна № 1228, ул. Тимуровцев, ул. Павлова, ул. Магистральная, Биофак, ул.Григория Алексеева, с/о Рябинушка, с/о Нефтяник, с/о Юбилей, ул. Хамита Ярми, ул. Романа Новопашина, ул. Дмитрия Коротчаева, ул. 1-я Школьная, ул. 1-я Молодежная, с/о Степное</t>
   </si>
   <si>
     <t>с/о Степное, 2-й Мостовой переулок, ул. Казаровская, Школа №52, ул. Хабибуллы Якина, Детский сад №127, Биофак, ул. Магистральная, ул. Павлова, ул. Тимуровцев, Автоколонна №1228, ул.Сеченова, II Заречный микрорайон, I Заречный микрорайон, ул. Мысовская, ул. 2-я Луговая, ул. Советская, гостиница Нефтяник, Администрация г. Тюмени, Центральный рынок, ул. Шиллера, ул. Малыгина, Медицинский колледж, Площадь Памяти,  ул. 30 лет Победы, ул. В. Гнаровской, Сквер Победы, ул. Депутатская, АЗС, ул. Революции, Детский сад №42, ЖК Апрель</t>
   </si>
   <si>
-    <t xml:space="preserve">ООО «Караван-Авто» 625059, Тюменская обл., г.Тюмень, ул.Щербакова д.172,                                            ИНН 7202143759 </t>
-  </si>
-  <si>
     <t>ул. Энтузиастов, Детский сад №62, Центр русской культуры, ул. Домостроителей, ул. Губкина, ул. Элеваторная, ул. Гилевская, Барабинская, Областная ГИБДД, з‑д Приборостроительный, Областная больница №1, Медицинский университет, Театральный центр Космос, м‑н Буратино, ДК Строитель, ул. Пермякова, III микрорайон, ул. Евгения Богдановича, ул. В. Гольцова, ул. Станислава Карнацевича, ул. Михаила Сперанского, ул. Прокопия Артамонова</t>
   </si>
   <si>
@@ -210,9 +189,6 @@
     <t>мкр. Южный, Школа №69, Городская юношеская библиотека, ул. Папанинцев, ул. Рабочая,Сквер Железнодорожников, ул. Мориса Тореза, Тюменский драматический театр, ул. Холодильная, Площадь Памяти, Театральный центр Космос, Школа №17, Кросно, ул. Воровского, з‑д Электрон, ЖБИ, Рабочий поселок, Управление Росгвардии, Ялуторовский тракт, ТЦ Лента, Гаражи, мкр. Лесной</t>
   </si>
   <si>
-    <t>ул. Созидателей - Тюменский индустриальный университет</t>
-  </si>
-  <si>
     <t>ул. Созидателей, ул. Обдорская, Проезд Ямбургский, ул. Андрея Бушуева, мкр. Ямальский 2, ул. Вадима Бованенко, ул. Губернская, ул. Александра Протозанова, мкр. Южный, ул. Бахарева, ул. Федюнинского, ул. Революции, ул. Дмитрия Менделеева, Сквер Льва Ровнина, Школа №92, ул. Евгения Богдановича, III микрорайон, Торговый центр, ул. Пермякова, Автовокзал, Пермякова, Севастопольская, Детская поликлиника №2, Тюменский индустриальный университет</t>
   </si>
   <si>
@@ -264,9 +240,6 @@
     <t>ул. Газопромысловая, ул. Академика Сахарова, Тарманы, ул. Игримская, ДК Торфяник, парк им. Гагарина, Геологоразведка, рынок Северный, ул. Ватутина, ул. Сеченова, Детский сад №160,  ул. Муравленко, ул. Газовиков, Детская поликлиника, I Заречный мкр., ул. Мысовская, ул. 2-я Луговая, ул. Советская, гостиница Нефтяник, Площадь Борцов Революции, Набережная, Строительный институт ТИУ, Детский сад №55, ул. Полевая, ул. Болотникова, Дом Обороны, ул. Аккумуляторная, з‑д Нефтемаш</t>
   </si>
   <si>
-    <t xml:space="preserve">ООО "Мос-Авто", 625049, Тюменская обл., г.Тюмень, проезд Воронинские горки, 142 стр. 4, оф. 8, ИНН 7203372060 </t>
-  </si>
-  <si>
     <t>ЖДВ – ул. Таллинская</t>
   </si>
   <si>
@@ -303,9 +276,6 @@
     <t>мкр. Суходольский, ЖК Юбилейный, Детский сад №141, Подъезд к развязке ул. Монтажников, ул. Воровского,  Сибнипигазстрой, з‑д Медоборудования, ДК Строитель, м‑н Буратино, Театральный центр Космос, Медицинский университет, ул. Котовского, Тюменский индустриальный университет, Областная больница №2, Студенческий городок, Мост Мельникайте, ул. Разведчика Кузнецова, Озеро Круглое, Лесопарк (центральный вход), Геологоразведка, рынок Северный, ул. Ватутина, Стоматологическая Поликлиника №1, Городская поликлиника №8</t>
   </si>
   <si>
-    <t>ООО «Караван-Авто» 625059, Тюменская обл., г.Тюмень, ул.Щербакова д.172,                                            ИНН 7202143759</t>
-  </si>
-  <si>
     <t>29д</t>
   </si>
   <si>
@@ -396,9 +366,6 @@
     <t>ул. Пролетарская, ул. Свободы, ул. Л. Толстого, Вечерняя школа №2, Строительный институт ТИУ, Музей, Университетская, Госбанк, Дворец творчества и спорта, ул. Первомайская, ул. Дзержинского, ул. 2-я Луговая, ул. Мысовская,  ул. Астраханская, I Заречный микрорайон, II Заречный микрорайон, Автоколонна №1228, Школа №9, микрорайон Югра, Детский сад №121, ул. Сосьвинская, Городская поликлиника №8, проезд Юганский, УМВД по г. Тюмени, ул. Ветеранов труда, з-д Керамзитовый, ул. Буровиков, Школа №45, п. ММС, ул. Голышева, с/о Мелиоратор, с/о Русское поле.</t>
   </si>
   <si>
-    <t>ИП Савельев Андрей Евгеньевич 625056, г.Тюмень, ул. Демократическая, 31 ИНН 720205152609</t>
-  </si>
-  <si>
     <t>СК Здоровье, Детская поликлиника, Филиал библиотеки им. А.С. Пушкина, ул. Муравленко, озеро Алебашево, Алебашевский базар, ул. Циолковского, ул. Даудельная, ул. Володарского, Сквер Немцова, Цветной бульвар, Центральный рынок, ул. Мориса Тореза, Сквер Железнодорожников, Универмаг, Университет путей сообщения, ул.Паровозная, Городская поликлиника №5, Администрация Тюменского района, Спортцентр Энерго, Универсальный рынок, Московский тракт, ул. Закалужская, ул. Панфиловцев, жилой район "Преображенский", ул. Александра Протозанова, ул. Губернская, ул. Заполярная, Сквер Вьюжный, Интеллект-Квартал, Аллея ветеранов Ямала, им. Вяхирева Рема Ивановича, Проезд Ямбургский, ул. Обдорская, ул. Созидателей</t>
   </si>
   <si>
@@ -417,9 +384,6 @@
     <t>ЖК Юбилейный, Театр Ангажемент, сквер Депутатов, мкр. Тюменский, III микрорайон, Торговый центр, ул. Пермякова, ДК Строитель, м-н Буратино, Театральный центр Космос, Медицинский университет, Областная больница №1, з-д Приборостроительный, Областная ГИБДД, Барабинская, ул. Гилёвская, Элеватор, ул. Губкина, ул. Домостроителей, Центр русской культуры, ул. Западносибирская, мкр. Тура, Школа №67, ул. Лесопарковая, ул. Мебельщиков, ул. Вересковая</t>
   </si>
   <si>
-    <t>ИП Шулепов Сергей Михайлович, 625017, г. Тюмень, ул. Черепанова, 76 ст. 6  ИНН 720400468814</t>
-  </si>
-  <si>
     <t>ул. Таллинская - ЖДВ</t>
   </si>
   <si>
@@ -429,9 +393,6 @@
     <t>ЖДВ, сквер Семена Пацко, ул. Смоленская, Цветной бульвар 1, Центральный рынок, ул. Мориса Тореза, ул. Шевченко, ул. Николая Чаплина, ул. Молодёжная, ул. Демьяна Бедного, ул. Салехардская, Гимназия №83, VI микрорайон, проезд 9 Мая, V мкр., мкр. Тюменский, Современник, ул. Олимпийская, проезд Монтажников, ул. Монтажников, мкр. Восточный, проезд Майский, ул. Народная, Поликлиника, Сквер Десантников, Восточный 3, ул. Теплотехников, ТЭЦ 2, ул. Боровская, ст. Войновка, ул. Таллинская</t>
   </si>
   <si>
-    <t>ИП Савельев Андрей Евгеньевич,625056, г.Тюмень, ул. Демократическая, 31 ИНН 720205152609</t>
-  </si>
-  <si>
     <t>Областная библиотека – Рабочий поселок</t>
   </si>
   <si>
@@ -441,9 +402,6 @@
     <t>Рабочий поселок, Тюменская домостроительная компания, з‑д Электрон, ул. Воровского, Сибнипигазстрой, з‑д Медоборудования, Автовокзал, Телецентр, ул. Энергетиков, Школа №7, Областная больница №1, ул. Одесская, Травматология,  ул. Харьковская, ул. Щорса, з‑д Судостроительный, ул. М. Горького, Бизнес-центр Петр Столыпин, Дом Печати, ул. Орджоникидзе, Дворец культуры Нефтяник, ул. Советская, гостиница Нефтяник, Администрация г. Тюмени, Областная научная библиотека</t>
   </si>
   <si>
-    <t xml:space="preserve">ООО "Мос-Авто", 625049, Тюменская обл., г.Тюмень ,проезд Воронинские горки, 142 стр. 4, оф. 8, ИНН 7203372060 </t>
-  </si>
-  <si>
     <t xml:space="preserve">ул. Возрождения – кафе Ивушка </t>
   </si>
   <si>
@@ -462,9 +420,6 @@
     <t>ул. Созидателей, ул. Обдорская, Проезд Ямбургский, "им. Вяхирева Рема Ивановича",  "Интеллект-квартал", "Сквер Вьюжный", ул. Василия Подшибякина, ул. Заполярная, ул. Вадима Бованенко, ул. Губернская, ул. Александра Протозанова, Многофункциональный центр, ул. Слободская, ул. Посадская, ул. Престольная, Больничный комплекс Нефтяник, ОБИЛ (основной корпус), Радиологический центр, Госпиталь "Мать и дитя", Многопрофильный клинический центр, ул. Прокопия Артамонова, Школа №92, Сквер Льва Ровнина, ул. Дмитрия Менделеева, ул. Депутатская, Сквер Победы, ул. Валерии Гнаровской, Кардиоцентр, ул. Рижская, Тюменский индустриальный университет, Областная больница №2, Студенческий городок, Мост Мельникайте, ул. Разведчика Кузнецова, Озеро Круглое, парк им. Гагарина, Западно-сибирский медицинский центр, "Школа №48 имени генерала Карбышева", ул. Судоремонтная, ул. Мусоргского, Тюмень Сити Молл,  ЖК Звездный городок</t>
   </si>
   <si>
-    <t>ИП Савельев Андрей Евгеньевич, 625056, г.Тюмень, ул. Демократическая, 31 ИНН 720205152609</t>
-  </si>
-  <si>
     <t>ЖК Звездный городок – ул. Таллинская</t>
   </si>
   <si>
@@ -630,9 +585,6 @@
     <t>ул. Высотная, ул. Ивана Крылова, ДК Поиск, поворот на Антипино, 4-км Старого Тобольского тракта, 3 км Старого Тобольского тракта, Поворот на конно-спортивную базу, Проезд до ул. Вологодская, з‑д Моторный, 2-й км Старого Тобольского тракта, з‑д Металлургический, Старый Тобольский тракт, Ялуторовский тракт, Управление Росгвардии, Рабочий поселок, Тюменская домостроительная компания, з‑д Электрон, ул. Воровского, Сибнипигазстрой, з‑д Медоборудования, ул. Пермякова, мкр. Тюменский, Современник, ул. Олимпийская, проезд Монтажников, мкр. Восточный, Школа №63, ул. Моторостроителей, Поликлиника, Сквер Десантников, Восточный 3, ул. Теплотехников, ТЭЦ 2, ул. Боровская, ст. Войновка, ул. Таллинская</t>
   </si>
   <si>
-    <t>ИП Савельев Андрей Евгеньевич, 625056, г.Тюмень, ул. Демократическая, 31, ИНН 720205152609</t>
-  </si>
-  <si>
     <t>с/о Степное – ДНТ Суходольное</t>
   </si>
   <si>
@@ -642,18 +594,12 @@
     <t>ДНТ Суходольное, ДНТ Суходольное 1, ДНТ Суходольное 2, с/о Лесная поляна, ул. Павла Шарова, Парк "Древо Жизни", ул. Звёздная, Стоматологическая поликлиника № 3, Школа № 56, ул. Николая Никитина, микрорайон Видный, мкр. Суходольский, МЖК, Школа №65, ул. Розы Трениной, сквер Депутатов, мкр. Тюменский, ТЦ Широтный, V мкр., ул. Николая Федорова, проезд 9 Мая, VI микрорайон, Гимназия №83, ул. Салехардская, ул. Демьяна Бедного, ул. Молодежная, ул. Колхозная, Информационно-библиотечный центр, Городская юношеская библиотека, ул. Папанинцев, ул. Рабочая, Сквер Железнодорожников, ул. Мориса Тореза, ул. Володарского, Детская поликлиника, ул. Даудельная,  ул. Циолковского, Алебашевский базар, ул. Эрвье, ул. Муравленко, Филиал библиотеки им. А.С. Пушкина, ул. Газовиков, Детская поликлиника, II Заречный микрорайон, Автоколонна №1228, ул. Тимуровцев, ул. Павлова, ул. Магистральная, Биофак, Детский сад №127, ул. Хабибуллы Якина, Школа №52,   ул. Казаровская, 2-й Мостовой переулок ,с/о Степное</t>
   </si>
   <si>
-    <t>ООО "Тюменьавтотранс", 625026, Тюменская обл., г. Тюмень, проезд Воронинские горки, 142 стр. 4, оф. 7, ИНН 7203372991</t>
-  </si>
-  <si>
     <t>Мыс – ул. Б. Комиссаров</t>
   </si>
   <si>
     <t>ул. Бакинских Комиссаров, Детский сад №110, ул. Пролетарская, ул. Пугачева, ул. Садовая, ул. Димитрова, Вечерняя школа №2, Строительный институт ТИУ, Музей, Университетская, Госбанк, Дворец творчества и спорта, ул. Первомайская, ул. Дзержинского, ул. 2-я Луговая, ул. Мысовская,  ул. Астраханская, I Заречный микрорайон, II Заречный микрорайон, ул. Сеченова, ул. Ачинская, ул. Дружбы, ул. Ватутина, рынок "Северный", сад Дружбы,  парк им. Гагарина, Западно-сибирский медицинский центр, "Школа №48 имени генерала Карбышева", ул. Судоремонтная, ул. Мусоргского, ул. Ершова, ул. Кулибина, Мыс</t>
   </si>
   <si>
-    <t>ИП Савельев Андрей Евгеньевич,625056, г.Тюмень, ул. Демократическая, 31, ИНН 720205152609</t>
-  </si>
-  <si>
     <t>ул. Энтузиастов, Детский сад №62, Центр русской культуры, ул. Домостроителей, ул. Губкина, ул. Элеваторная, ул. Гилевская, Барабинская, Областная ГИБДД, ул. Одесская, Областная больница №2, Тюменский индустриальный университет, ул. Рижская, Площадь Памяти, Площадь Памяти, ул. Таймырская, ул. Малыгина, ул. Шиллера, ул. Мориса Тореза,Сквер Железнодорожников, Универмаг, Университет путей сообщения,ул. Паровозная, Городская поликлиника №5, Администрация Тюменского района, Спортцентр Энерго, Универсальный рынок, Московский тракт, ул. Кремлевская, ЖК Плеханово</t>
   </si>
   <si>
@@ -669,9 +615,6 @@
     <t>ул. Народная, Поликлиника, ул. Моторостроителей, Театр Ангажемент, Городская поликлиника №17, ул. Суходольская, ул. Василия Гольцова, Школа №92, Сквер Льва Ровнина, ул. Дмитрия Менделеева, ул. Депутатская, Сквер Победы, ул. Валерии Гнаровской, Газпром, ул. Холодильная, ул. Максима Горького, площадь Центральная, ул. Первомайская, ул. Смоленская, ЖДВ</t>
   </si>
   <si>
-    <t>ИП Савельев Андрей Евгеньевич,625056, г.Тюмень, ул. Демократическая, 31,  ИНН 720205152609</t>
-  </si>
-  <si>
     <t>ул. Газопромысловая – МО МВД России "Тюменский"</t>
   </si>
   <si>
@@ -937,9 +880,6 @@
   </si>
   <si>
     <t>с/о Липовый остров, ул. 6-я Западная, с/о Поле чудес, с/о Березняки, ул. Клубничная, Парк Пограничников, Детский сад №127, Биофак, ул. Магистральная, ул. Павлова, ул. Тимуровцев, Автоколонна №1228, ул. Сеченова, II Заречный микрорайон, СК Здоровье, I Заречный микрорайон, ул. Мысовская, ул. 2-я Луговая, ул. Советская, гостиница "Нефтяник", Администрация города Тюмени, Областная научная библиотека</t>
-  </si>
-  <si>
-    <t>44,75 (37,27)</t>
   </si>
   <si>
     <t>ЖК Правобережный, ул.Щорса, з-д Судостроительный, ул. М. Горького, Спорткомплекс Строймаш, Областное управление МЧС, Тюменский дратический театр, ул. Холодильная, Площадь Памяти, Рыбокомбинат, Горводоканал, Озерные аркады, Березовая роща, ул. Н. Зелинского, Сквер Льва Ровнина,  школа №92, ул. П. Артамонова, ул. Восточная, ул. Звездная, Парк "Дерево жизни", ул. В.Трофимовой, Школа № 65, Стоматологическая поликлиника № 3, ул. А. Митинского, ул. Восточная</t>
@@ -1368,6 +1308,60 @@
   </si>
   <si>
     <t>НСАОО</t>
+  </si>
+  <si>
+    <t>ул. Созидателей - ТИУ</t>
+  </si>
+  <si>
+    <t>56.56</t>
+  </si>
+  <si>
+    <t>АО "ТПАТП №1" 625019
+ИНН 7203193689</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ООО "Тюменьавтотранс"
+ИНН 7203372991 </t>
+  </si>
+  <si>
+    <t>ООО "Тюменьавтотранс"
+ИНН 7203372991</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ИП Шулепов Сергей Михайлович 625017
+ИНН 720400468814 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ООО «Караван-Авто» 625059
+ИНН 7202143759 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ООО "Мос-Авто"
+ИНН 7203372060 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ООО "Мос-Авто", 625049
+ИНН 7203372060 </t>
+  </si>
+  <si>
+    <t>ООО «Караван-Авто» 625059
+ИНН 7202143759</t>
+  </si>
+  <si>
+    <t>ИП Савельев Андрей Евгеньевич 625056
+ИНН 720205152609</t>
+  </si>
+  <si>
+    <t>ИП Шулепов Сергей Михайлович, 625017
+ИНН 720400468814</t>
+  </si>
+  <si>
+    <t>ИП Савельев Андрей Евгеньевич,625056
+ИНН 720205152609</t>
+  </si>
+  <si>
+    <t>ИП Савельев Андрей Евгеньевич, 625056
+ИНН 720205152609</t>
   </si>
 </sst>
 </file>
@@ -1740,11 +1734,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243FB209-417C-44A1-9773-2C6487EF2D51}">
   <dimension ref="A1:M98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.109375" style="1" bestFit="1" customWidth="1"/>
@@ -1761,24 +1755,24 @@
     <col min="14" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>331</v>
+        <v>311</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>332</v>
+        <v>312</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>333</v>
+        <v>313</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>334</v>
+        <v>314</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>5</v>
@@ -1790,10 +1784,10 @@
         <v>2</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>445</v>
+        <v>425</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>3</v>
@@ -1802,7 +1796,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1810,13 +1804,13 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>311</v>
+        <v>291</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>335</v>
+        <v>315</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>335</v>
+        <v>315</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>7</v>
@@ -1836,34 +1830,34 @@
       <c r="L2" s="3">
         <v>40796</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>14</v>
+      <c r="I3" s="1">
+        <v>49.59</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>9</v>
@@ -1874,11 +1868,11 @@
       <c r="L3" s="3">
         <v>44197</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M3" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1886,22 +1880,22 @@
         <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="I4" s="1" t="s">
-        <v>18</v>
+        <v>428</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>9</v>
@@ -1912,11 +1906,11 @@
       <c r="L4" s="3">
         <v>41666</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M4" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1924,19 +1918,19 @@
         <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>339</v>
+        <v>319</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>360</v>
+        <v>340</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I5" s="1">
         <v>18.34</v>
@@ -1950,31 +1944,31 @@
       <c r="L5" s="3">
         <v>40796</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="M5" s="2" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="I6" s="1">
         <v>23.35</v>
@@ -1988,11 +1982,11 @@
       <c r="L6" s="3">
         <v>44197</v>
       </c>
-      <c r="M6" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M6" s="2" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2000,19 +1994,19 @@
         <v>9</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>313</v>
+        <v>293</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>340</v>
+        <v>320</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>386</v>
+        <v>366</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="I7" s="1">
         <v>32.49</v>
@@ -2026,11 +2020,11 @@
       <c r="L7" s="3">
         <v>40796</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M7" s="2" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2038,19 +2032,19 @@
         <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>314</v>
+        <v>294</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>341</v>
+        <v>321</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>387</v>
+        <v>367</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="I8" s="1">
         <v>36.020000000000003</v>
@@ -2064,11 +2058,11 @@
       <c r="L8" s="3">
         <v>40796</v>
       </c>
-      <c r="M8" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M8" s="2" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2076,19 +2070,19 @@
         <v>9</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>315</v>
+        <v>295</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>342</v>
+        <v>322</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>388</v>
+        <v>368</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="I9" s="1">
         <v>23.58</v>
@@ -2102,11 +2096,11 @@
       <c r="L9" s="3">
         <v>41091</v>
       </c>
-      <c r="M9" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M9" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2114,19 +2108,19 @@
         <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>343</v>
+        <v>323</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>340</v>
+        <v>320</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="I10" s="1">
         <v>46.29</v>
@@ -2140,11 +2134,11 @@
       <c r="L10" s="3">
         <v>42065</v>
       </c>
-      <c r="M10" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M10" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2152,19 +2146,19 @@
         <v>9</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>339</v>
+        <v>319</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>389</v>
+        <v>369</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="I11" s="1">
         <v>32.96</v>
@@ -2178,11 +2172,11 @@
       <c r="L11" s="3">
         <v>40796</v>
       </c>
-      <c r="M11" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M11" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2190,19 +2184,19 @@
         <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>344</v>
+        <v>324</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>390</v>
+        <v>370</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="I12" s="1">
         <v>38.700000000000003</v>
@@ -2216,11 +2210,11 @@
       <c r="L12" s="3">
         <v>40796</v>
       </c>
-      <c r="M12" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M12" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2228,19 +2222,19 @@
         <v>9</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>345</v>
+        <v>325</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>391</v>
+        <v>371</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="I13" s="1">
         <v>29.95</v>
@@ -2254,31 +2248,31 @@
       <c r="L13" s="3">
         <v>40796</v>
       </c>
-      <c r="M13" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M13" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>346</v>
+        <v>326</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>391</v>
+        <v>371</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="I14" s="1">
         <v>45.29</v>
@@ -2292,11 +2286,11 @@
       <c r="L14" s="3">
         <v>44197</v>
       </c>
-      <c r="M14" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M14" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2304,19 +2298,19 @@
         <v>9</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>347</v>
+        <v>327</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>352</v>
+        <v>332</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="I15" s="1">
         <v>27.74</v>
@@ -2330,11 +2324,11 @@
       <c r="L15" s="3">
         <v>40796</v>
       </c>
-      <c r="M15" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M15" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2342,19 +2336,19 @@
         <v>9</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>348</v>
+        <v>328</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>392</v>
+        <v>372</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="I16" s="1">
         <v>33.24</v>
@@ -2368,11 +2362,11 @@
       <c r="L16" s="3">
         <v>40796</v>
       </c>
-      <c r="M16" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M16" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2380,19 +2374,19 @@
         <v>9</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>337</v>
+        <v>317</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>386</v>
+        <v>366</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="I17" s="1">
         <v>38.15</v>
@@ -2406,11 +2400,11 @@
       <c r="L17" s="3">
         <v>40796</v>
       </c>
-      <c r="M17" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M17" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2418,19 +2412,19 @@
         <v>9</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>61</v>
+        <v>427</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>349</v>
+        <v>329</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>393</v>
+        <v>373</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="I18" s="1">
         <v>34.409999999999997</v>
@@ -2444,11 +2438,11 @@
       <c r="L18" s="3">
         <v>43101</v>
       </c>
-      <c r="M18" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M18" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2456,19 +2450,19 @@
         <v>9</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>316</v>
+        <v>296</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>350</v>
+        <v>330</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>394</v>
+        <v>374</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="I19" s="1">
         <v>41.4</v>
@@ -2482,31 +2476,31 @@
       <c r="L19" s="3">
         <v>40796</v>
       </c>
-      <c r="M19" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M19" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>317</v>
+        <v>297</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>350</v>
+        <v>330</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>395</v>
+        <v>375</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="I20" s="1">
         <v>40.08</v>
@@ -2520,11 +2514,11 @@
       <c r="L20" s="3">
         <v>44197</v>
       </c>
-      <c r="M20" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M20" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -2532,19 +2526,19 @@
         <v>9</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>351</v>
+        <v>331</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>396</v>
+        <v>376</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="I21" s="1">
         <v>27.08</v>
@@ -2558,11 +2552,11 @@
       <c r="L21" s="3">
         <v>40796</v>
       </c>
-      <c r="M21" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M21" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2570,19 +2564,19 @@
         <v>9</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>352</v>
+        <v>332</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="I22" s="1">
         <v>23.63</v>
@@ -2596,11 +2590,11 @@
       <c r="L22" s="3">
         <v>40796</v>
       </c>
-      <c r="M22" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M22" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2608,19 +2602,19 @@
         <v>9</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>353</v>
+        <v>333</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>398</v>
+        <v>378</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="I23" s="1">
         <v>23.57</v>
@@ -2634,11 +2628,11 @@
       <c r="L23" s="3">
         <v>41666</v>
       </c>
-      <c r="M23" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M23" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>24</v>
       </c>
@@ -2646,19 +2640,19 @@
         <v>9</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>354</v>
+        <v>334</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>351</v>
+        <v>331</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="I24" s="1">
         <v>30.85</v>
@@ -2672,11 +2666,11 @@
       <c r="L24" s="3">
         <v>41810</v>
       </c>
-      <c r="M24" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M24" s="2" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>25</v>
       </c>
@@ -2684,19 +2678,19 @@
         <v>9</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>352</v>
+        <v>332</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>343</v>
+        <v>323</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="I25" s="1">
         <v>28.52</v>
@@ -2710,11 +2704,11 @@
       <c r="L25" s="3">
         <v>40796</v>
       </c>
-      <c r="M25" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M25" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>26</v>
       </c>
@@ -2722,19 +2716,19 @@
         <v>9</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>355</v>
+        <v>335</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>366</v>
+        <v>346</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="I26" s="1">
         <v>9.8000000000000007</v>
@@ -2748,11 +2742,11 @@
       <c r="L26" s="3">
         <v>40796</v>
       </c>
-      <c r="M26" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M26" s="2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>27</v>
       </c>
@@ -2760,19 +2754,19 @@
         <v>9</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>356</v>
+        <v>336</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>352</v>
+        <v>332</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="I27" s="1">
         <v>23.54</v>
@@ -2786,11 +2780,11 @@
       <c r="L27" s="3">
         <v>40796</v>
       </c>
-      <c r="M27" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M27" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>29</v>
       </c>
@@ -2798,19 +2792,19 @@
         <v>9</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>357</v>
+        <v>337</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>399</v>
+        <v>379</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="I28" s="1">
         <v>31.95</v>
@@ -2824,31 +2818,31 @@
       <c r="L28" s="3">
         <v>40796</v>
       </c>
-      <c r="M28" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M28" s="2" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>358</v>
+        <v>338</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>399</v>
+        <v>379</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="I29" s="1">
         <v>39.4</v>
@@ -2862,11 +2856,11 @@
       <c r="L29" s="3">
         <v>44197</v>
       </c>
-      <c r="M29" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M29" s="2" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>30</v>
       </c>
@@ -2874,19 +2868,19 @@
         <v>9</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>350</v>
+        <v>330</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>382</v>
+        <v>362</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="I30" s="1">
         <v>34.21</v>
@@ -2900,11 +2894,11 @@
       <c r="L30" s="3">
         <v>40796</v>
       </c>
-      <c r="M30" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M30" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>31</v>
       </c>
@@ -2912,19 +2906,19 @@
         <v>9</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>339</v>
+        <v>319</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>340</v>
+        <v>320</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="I31" s="1">
         <v>21.83</v>
@@ -2938,11 +2932,11 @@
       <c r="L31" s="3">
         <v>40796</v>
       </c>
-      <c r="M31" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M31" s="2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>32</v>
       </c>
@@ -2950,19 +2944,19 @@
         <v>9</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>352</v>
+        <v>332</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>400</v>
+        <v>380</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="I32" s="1">
         <v>24.95</v>
@@ -2976,11 +2970,11 @@
       <c r="L32" s="3">
         <v>40796</v>
       </c>
-      <c r="M32" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M32" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>33</v>
       </c>
@@ -2988,19 +2982,19 @@
         <v>9</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>352</v>
+        <v>332</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>401</v>
+        <v>381</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="I33" s="1">
         <v>35.21</v>
@@ -3014,11 +3008,11 @@
       <c r="L33" s="3">
         <v>40796</v>
       </c>
-      <c r="M33" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M33" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>34</v>
       </c>
@@ -3026,19 +3020,19 @@
         <v>9</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>352</v>
+        <v>332</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>361</v>
+        <v>341</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="I34" s="1">
         <v>30.54</v>
@@ -3052,11 +3046,11 @@
       <c r="L34" s="3">
         <v>40796</v>
       </c>
-      <c r="M34" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M34" s="2" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>35</v>
       </c>
@@ -3064,19 +3058,19 @@
         <v>9</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>359</v>
+        <v>339</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>339</v>
+        <v>319</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="I35" s="1">
         <v>20.87</v>
@@ -3090,11 +3084,11 @@
       <c r="L35" s="3">
         <v>43831</v>
       </c>
-      <c r="M35" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M35" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>36</v>
       </c>
@@ -3102,19 +3096,19 @@
         <v>9</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>339</v>
+        <v>319</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="I36" s="1">
         <v>46.73</v>
@@ -3128,31 +3122,31 @@
       <c r="L36" s="3">
         <v>40796</v>
       </c>
-      <c r="M36" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M36" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>339</v>
+        <v>319</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="I37" s="1">
         <v>41.16</v>
@@ -3166,11 +3160,11 @@
       <c r="L37" s="3">
         <v>44197</v>
       </c>
-      <c r="M37" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M37" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -3178,19 +3172,19 @@
         <v>9</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>321</v>
+        <v>301</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>360</v>
+        <v>340</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>404</v>
+        <v>384</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="I38" s="1">
         <v>29.53</v>
@@ -3204,11 +3198,11 @@
       <c r="L38" s="3">
         <v>40796</v>
       </c>
-      <c r="M38" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M38" s="2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>39</v>
       </c>
@@ -3216,19 +3210,19 @@
         <v>9</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>322</v>
+        <v>302</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>353</v>
+        <v>333</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>349</v>
+        <v>329</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="I39" s="1">
         <v>41.61</v>
@@ -3242,11 +3236,11 @@
       <c r="L39" s="3">
         <v>40796</v>
       </c>
-      <c r="M39" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M39" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>40</v>
       </c>
@@ -3254,19 +3248,19 @@
         <v>9</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>323</v>
+        <v>303</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>361</v>
+        <v>341</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>364</v>
+        <v>344</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="I40" s="1">
         <v>31.85</v>
@@ -3280,11 +3274,11 @@
       <c r="L40" s="3">
         <v>41810</v>
       </c>
-      <c r="M40" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M40" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>41</v>
       </c>
@@ -3292,19 +3286,19 @@
         <v>9</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>324</v>
+        <v>304</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>362</v>
+        <v>342</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>405</v>
+        <v>385</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="I41" s="1">
         <v>30.48</v>
@@ -3318,11 +3312,11 @@
       <c r="L41" s="3">
         <v>43831</v>
       </c>
-      <c r="M41" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M41" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>42</v>
       </c>
@@ -3330,19 +3324,19 @@
         <v>9</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>343</v>
+        <v>323</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>406</v>
+        <v>386</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="I42" s="1">
         <v>29.93</v>
@@ -3356,11 +3350,11 @@
       <c r="L42" s="3">
         <v>41827</v>
       </c>
-      <c r="M42" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M42" s="2" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>43</v>
       </c>
@@ -3368,19 +3362,19 @@
         <v>9</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>355</v>
+        <v>335</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>345</v>
+        <v>325</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="I43" s="1">
         <v>23.87</v>
@@ -3394,11 +3388,11 @@
       <c r="L43" s="3">
         <v>40796</v>
       </c>
-      <c r="M43" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M43" s="2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>44</v>
       </c>
@@ -3406,19 +3400,19 @@
         <v>9</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>363</v>
+        <v>343</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>407</v>
+        <v>387</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="I44" s="1">
         <v>31.62</v>
@@ -3432,11 +3426,11 @@
       <c r="L44" s="3">
         <v>40796</v>
       </c>
-      <c r="M44" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M44" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>45</v>
       </c>
@@ -3444,19 +3438,19 @@
         <v>9</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>364</v>
+        <v>344</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>349</v>
+        <v>329</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="I45" s="1">
         <v>55</v>
@@ -3470,11 +3464,11 @@
       <c r="L45" s="3">
         <v>40796</v>
       </c>
-      <c r="M45" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M45" s="2" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>46</v>
       </c>
@@ -3482,19 +3476,19 @@
         <v>9</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>364</v>
+        <v>344</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>343</v>
+        <v>323</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="I46" s="1">
         <v>43.66</v>
@@ -3508,11 +3502,11 @@
       <c r="L46" s="3">
         <v>40796</v>
       </c>
-      <c r="M46" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M46" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>47</v>
       </c>
@@ -3520,19 +3514,19 @@
         <v>9</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>365</v>
+        <v>345</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>408</v>
+        <v>388</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="I47" s="1">
         <v>32.33</v>
@@ -3546,31 +3540,31 @@
       <c r="L47" s="3">
         <v>41709</v>
       </c>
-      <c r="M47" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M47" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>365</v>
+        <v>345</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>409</v>
+        <v>389</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="I48" s="1">
         <v>34.409999999999997</v>
@@ -3584,11 +3578,11 @@
       <c r="L48" s="3">
         <v>43831</v>
       </c>
-      <c r="M48" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M48" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -3596,19 +3590,19 @@
         <v>9</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>360</v>
+        <v>340</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>410</v>
+        <v>390</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="I49" s="1">
         <v>32.58</v>
@@ -3622,11 +3616,11 @@
       <c r="L49" s="3">
         <v>40796</v>
       </c>
-      <c r="M49" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M49" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -3634,19 +3628,19 @@
         <v>9</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>366</v>
+        <v>346</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>411</v>
+        <v>391</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="I50" s="1">
         <v>36.880000000000003</v>
@@ -3660,11 +3654,11 @@
       <c r="L50" s="3">
         <v>40796</v>
       </c>
-      <c r="M50" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M50" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -3672,19 +3666,19 @@
         <v>9</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>367</v>
+        <v>347</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>378</v>
+        <v>358</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="I51" s="1">
         <v>21.55</v>
@@ -3698,11 +3692,11 @@
       <c r="L51" s="3">
         <v>40796</v>
       </c>
-      <c r="M51" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M51" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -3710,19 +3704,19 @@
         <v>9</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>360</v>
+        <v>340</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>412</v>
+        <v>392</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="I52" s="1">
         <v>44.04</v>
@@ -3736,31 +3730,31 @@
       <c r="L52" s="3">
         <v>40983</v>
       </c>
-      <c r="M52" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M52" s="2" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>325</v>
+        <v>305</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>368</v>
+        <v>348</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>413</v>
+        <v>393</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="I53" s="1">
         <v>49.37</v>
@@ -3774,11 +3768,11 @@
       <c r="L53" s="3">
         <v>44197</v>
       </c>
-      <c r="M53" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M53" s="2" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -3786,19 +3780,19 @@
         <v>9</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>369</v>
+        <v>349</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>414</v>
+        <v>394</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="I54" s="1">
         <v>16.11</v>
@@ -3812,11 +3806,11 @@
       <c r="L54" s="3">
         <v>40796</v>
       </c>
-      <c r="M54" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M54" s="2" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -3824,19 +3818,19 @@
         <v>9</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>370</v>
+        <v>350</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>364</v>
+        <v>344</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="I55" s="1">
         <v>43.31</v>
@@ -3850,11 +3844,11 @@
       <c r="L55" s="3">
         <v>40796</v>
       </c>
-      <c r="M55" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M55" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -3862,19 +3856,19 @@
         <v>9</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>364</v>
+        <v>344</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>415</v>
+        <v>395</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="I56" s="1">
         <v>44.76</v>
@@ -3888,31 +3882,31 @@
       <c r="L56" s="3">
         <v>40796</v>
       </c>
-      <c r="M56" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M56" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>364</v>
+        <v>344</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>344</v>
+        <v>324</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="I57" s="1">
         <v>53.91</v>
@@ -3926,11 +3920,11 @@
       <c r="L57" s="3">
         <v>44197</v>
       </c>
-      <c r="M57" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M57" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>55</v>
       </c>
@@ -3938,19 +3932,19 @@
         <v>9</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>338</v>
+        <v>318</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>376</v>
+        <v>356</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="I58" s="1">
         <v>42.73</v>
@@ -3964,11 +3958,11 @@
       <c r="L58" s="3">
         <v>41575</v>
       </c>
-      <c r="M58" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M58" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -3976,19 +3970,19 @@
         <v>9</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>343</v>
+        <v>323</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>416</v>
+        <v>396</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="I59" s="1">
         <v>34.03</v>
@@ -4002,11 +3996,11 @@
       <c r="L59" s="3">
         <v>40796</v>
       </c>
-      <c r="M59" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M59" s="2" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>60</v>
       </c>
@@ -4014,19 +4008,19 @@
         <v>9</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>371</v>
+        <v>351</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>417</v>
+        <v>397</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="I60" s="1">
         <v>36.630000000000003</v>
@@ -4040,11 +4034,11 @@
       <c r="L60" s="3">
         <v>42065</v>
       </c>
-      <c r="M60" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M60" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>62</v>
       </c>
@@ -4052,19 +4046,19 @@
         <v>9</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>372</v>
+        <v>352</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>382</v>
+        <v>362</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="I61" s="1">
         <v>37.35</v>
@@ -4078,11 +4072,11 @@
       <c r="L61" s="3">
         <v>40796</v>
       </c>
-      <c r="M61" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M61" s="2" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>63</v>
       </c>
@@ -4090,19 +4084,19 @@
         <v>9</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>373</v>
+        <v>353</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>418</v>
+        <v>398</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="I62" s="1">
         <v>62.29</v>
@@ -4116,11 +4110,11 @@
       <c r="L62" s="3">
         <v>41883</v>
       </c>
-      <c r="M62" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M62" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>64</v>
       </c>
@@ -4128,19 +4122,19 @@
         <v>9</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>343</v>
+        <v>323</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>419</v>
+        <v>399</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="I63" s="1">
         <v>40.67</v>
@@ -4154,11 +4148,11 @@
       <c r="L63" s="3">
         <v>40796</v>
       </c>
-      <c r="M63" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M63" s="2" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>65</v>
       </c>
@@ -4166,19 +4160,19 @@
         <v>9</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>374</v>
+        <v>354</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>420</v>
+        <v>400</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="I64" s="1">
         <v>54.39</v>
@@ -4192,11 +4186,11 @@
       <c r="L64" s="3">
         <v>40796</v>
       </c>
-      <c r="M64" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M64" s="2" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>68</v>
       </c>
@@ -4204,19 +4198,19 @@
         <v>9</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>206</v>
+        <v>189</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>375</v>
+        <v>355</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>421</v>
+        <v>401</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>310</v>
+        <v>290</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
       <c r="I65" s="1">
         <v>32.9</v>
@@ -4230,11 +4224,11 @@
       <c r="L65" s="3">
         <v>40796</v>
       </c>
-      <c r="M65" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M65" s="2" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>70</v>
       </c>
@@ -4242,19 +4236,19 @@
         <v>9</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>327</v>
+        <v>307</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>342</v>
+        <v>322</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>422</v>
+        <v>402</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="I66" s="1">
         <v>29.9</v>
@@ -4268,11 +4262,11 @@
       <c r="L66" s="3">
         <v>41813</v>
       </c>
-      <c r="M66" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M66" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>73</v>
       </c>
@@ -4280,19 +4274,19 @@
         <v>9</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>352</v>
+        <v>332</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>423</v>
+        <v>403</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="I67" s="1">
         <v>28.69</v>
@@ -4306,11 +4300,11 @@
       <c r="L67" s="3">
         <v>44197</v>
       </c>
-      <c r="M67" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M67" s="2" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>76</v>
       </c>
@@ -4318,19 +4312,19 @@
         <v>9</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>351</v>
+        <v>331</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>424</v>
+        <v>404</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>216</v>
+        <v>197</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="I68" s="1">
         <v>46.01</v>
@@ -4344,11 +4338,11 @@
       <c r="L68" s="3">
         <v>40796</v>
       </c>
-      <c r="M68" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M68" s="2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>79</v>
       </c>
@@ -4356,19 +4350,19 @@
         <v>9</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>350</v>
+        <v>330</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>414</v>
+        <v>394</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
       <c r="I69" s="1">
         <v>30.86</v>
@@ -4382,11 +4376,11 @@
       <c r="L69" s="3">
         <v>40796</v>
       </c>
-      <c r="M69" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M69" s="2" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>83</v>
       </c>
@@ -4394,19 +4388,19 @@
         <v>9</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>221</v>
+        <v>202</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>352</v>
+        <v>332</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>378</v>
+        <v>358</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>223</v>
+        <v>204</v>
       </c>
       <c r="I70" s="1">
         <v>27.07</v>
@@ -4420,11 +4414,11 @@
       <c r="L70" s="3">
         <v>41883</v>
       </c>
-      <c r="M70" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M70" s="2" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>84</v>
       </c>
@@ -4432,19 +4426,19 @@
         <v>9</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>376</v>
+        <v>356</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>378</v>
+        <v>358</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>225</v>
+        <v>206</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>226</v>
+        <v>207</v>
       </c>
       <c r="I71" s="1">
         <v>44.71</v>
@@ -4458,11 +4452,11 @@
       <c r="L71" s="3">
         <v>40796</v>
       </c>
-      <c r="M71" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M71" s="2" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>85</v>
       </c>
@@ -4470,19 +4464,19 @@
         <v>9</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>377</v>
+        <v>357</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>425</v>
+        <v>405</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
       <c r="I72" s="1">
         <v>45.43</v>
@@ -4496,11 +4490,11 @@
       <c r="L72" s="3">
         <v>40796</v>
       </c>
-      <c r="M72" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M72" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>86</v>
       </c>
@@ -4508,19 +4502,19 @@
         <v>9</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>373</v>
+        <v>353</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>378</v>
+        <v>358</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>231</v>
+        <v>212</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
       <c r="I73" s="1">
         <v>39.79</v>
@@ -4534,11 +4528,11 @@
       <c r="L73" s="3">
         <v>40796</v>
       </c>
-      <c r="M73" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M73" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>88</v>
       </c>
@@ -4546,19 +4540,19 @@
         <v>9</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>364</v>
+        <v>344</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>426</v>
+        <v>406</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>235</v>
+        <v>216</v>
       </c>
       <c r="I74" s="1">
         <v>40.25</v>
@@ -4572,11 +4566,11 @@
       <c r="L74" s="3">
         <v>41946</v>
       </c>
-      <c r="M74" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M74" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>89</v>
       </c>
@@ -4584,19 +4578,19 @@
         <v>9</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>384</v>
+        <v>364</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>352</v>
+        <v>332</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>349</v>
+        <v>329</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>236</v>
+        <v>217</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>237</v>
+        <v>218</v>
       </c>
       <c r="I75" s="1">
         <v>29.39</v>
@@ -4610,11 +4604,11 @@
       <c r="L75" s="3">
         <v>40796</v>
       </c>
-      <c r="M75" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M75" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>91</v>
       </c>
@@ -4622,19 +4616,19 @@
         <v>9</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>378</v>
+        <v>358</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>427</v>
+        <v>407</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>239</v>
+        <v>220</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>240</v>
+        <v>221</v>
       </c>
       <c r="I76" s="1">
         <v>28.8</v>
@@ -4648,11 +4642,11 @@
       <c r="L76" s="3">
         <v>40796</v>
       </c>
-      <c r="M76" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M76" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>96</v>
       </c>
@@ -4660,19 +4654,19 @@
         <v>9</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>241</v>
+        <v>222</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>373</v>
+        <v>353</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>414</v>
+        <v>394</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>242</v>
+        <v>223</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="I77" s="1">
         <v>23.01</v>
@@ -4686,11 +4680,11 @@
       <c r="L77" s="3">
         <v>40796</v>
       </c>
-      <c r="M77" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M77" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>98</v>
       </c>
@@ -4698,19 +4692,19 @@
         <v>9</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>244</v>
+        <v>225</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>379</v>
+        <v>359</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>428</v>
+        <v>408</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>245</v>
+        <v>226</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>246</v>
+        <v>227</v>
       </c>
       <c r="I78" s="1">
         <v>40.369999999999997</v>
@@ -4724,11 +4718,11 @@
       <c r="L78" s="3">
         <v>40796</v>
       </c>
-      <c r="M78" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M78" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>99</v>
       </c>
@@ -4736,19 +4730,19 @@
         <v>9</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>247</v>
+        <v>228</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>355</v>
+        <v>335</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>429</v>
+        <v>409</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="I79" s="1">
         <v>45.56</v>
@@ -4762,11 +4756,11 @@
       <c r="L79" s="3">
         <v>40796</v>
       </c>
-      <c r="M79" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M79" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>100</v>
       </c>
@@ -4774,19 +4768,19 @@
         <v>9</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>250</v>
+        <v>231</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>339</v>
+        <v>319</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>429</v>
+        <v>409</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>251</v>
+        <v>232</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>252</v>
+        <v>233</v>
       </c>
       <c r="I80" s="1">
         <v>29.84</v>
@@ -4800,31 +4794,31 @@
       <c r="L80" s="3">
         <v>40796</v>
       </c>
-      <c r="M80" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M80" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>254</v>
+        <v>235</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>380</v>
+        <v>360</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>430</v>
+        <v>410</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>255</v>
+        <v>236</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>256</v>
+        <v>237</v>
       </c>
       <c r="I81" s="1">
         <v>37.36</v>
@@ -4838,11 +4832,11 @@
       <c r="L81" s="3">
         <v>40796</v>
       </c>
-      <c r="M81" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M81" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>120</v>
       </c>
@@ -4850,19 +4844,19 @@
         <v>9</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>257</v>
+        <v>238</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>381</v>
+        <v>361</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>431</v>
+        <v>411</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>258</v>
+        <v>239</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>259</v>
+        <v>240</v>
       </c>
       <c r="I82" s="1">
         <v>52.02</v>
@@ -4876,31 +4870,31 @@
       <c r="L82" s="3">
         <v>40796</v>
       </c>
-      <c r="M82" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M82" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>328</v>
+        <v>308</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>353</v>
+        <v>333</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>432</v>
+        <v>412</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>261</v>
+        <v>242</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>262</v>
+        <v>243</v>
       </c>
       <c r="I83" s="1">
         <v>34.94</v>
@@ -4914,11 +4908,11 @@
       <c r="L83" s="3">
         <v>44197</v>
       </c>
-      <c r="M83" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M83" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>121</v>
       </c>
@@ -4926,19 +4920,19 @@
         <v>9</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>263</v>
+        <v>244</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>352</v>
+        <v>332</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>433</v>
+        <v>413</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>264</v>
+        <v>245</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>265</v>
+        <v>246</v>
       </c>
       <c r="I84" s="1">
         <v>26.11</v>
@@ -4952,11 +4946,11 @@
       <c r="L84" s="3">
         <v>40796</v>
       </c>
-      <c r="M84" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M84" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>128</v>
       </c>
@@ -4964,19 +4958,19 @@
         <v>9</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>266</v>
+        <v>247</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>373</v>
+        <v>353</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>434</v>
+        <v>414</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>268</v>
+        <v>249</v>
       </c>
       <c r="I85" s="1">
         <v>39.65</v>
@@ -4990,31 +4984,31 @@
       <c r="L85" s="3">
         <v>40796</v>
       </c>
-      <c r="M85" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M85" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>269</v>
+        <v>250</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>270</v>
+        <v>251</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>373</v>
+        <v>353</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>435</v>
+        <v>415</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>271</v>
+        <v>252</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>272</v>
+        <v>253</v>
       </c>
       <c r="I86" s="1">
         <v>56.01</v>
@@ -5028,11 +5022,11 @@
       <c r="L86" s="3">
         <v>40796</v>
       </c>
-      <c r="M86" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M86" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>135</v>
       </c>
@@ -5040,19 +5034,19 @@
         <v>9</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>273</v>
+        <v>254</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>339</v>
+        <v>319</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>436</v>
+        <v>416</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>274</v>
+        <v>255</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>275</v>
+        <v>256</v>
       </c>
       <c r="I87" s="1">
         <v>37.56</v>
@@ -5066,11 +5060,11 @@
       <c r="L87" s="3">
         <v>40796</v>
       </c>
-      <c r="M87" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M87" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>140</v>
       </c>
@@ -5078,19 +5072,19 @@
         <v>9</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>276</v>
+        <v>257</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>339</v>
+        <v>319</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>437</v>
+        <v>417</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>277</v>
+        <v>258</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>278</v>
+        <v>259</v>
       </c>
       <c r="I88" s="1">
         <v>61.45</v>
@@ -5104,11 +5098,11 @@
       <c r="L88" s="3">
         <v>40796</v>
       </c>
-      <c r="M88" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="89" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M88" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>144</v>
       </c>
@@ -5116,19 +5110,19 @@
         <v>9</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>279</v>
+        <v>260</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>373</v>
+        <v>353</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>438</v>
+        <v>418</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>280</v>
+        <v>261</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
       <c r="I89" s="1">
         <v>49.07</v>
@@ -5142,11 +5136,11 @@
       <c r="L89" s="3">
         <v>40796</v>
       </c>
-      <c r="M89" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M89" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>145</v>
       </c>
@@ -5154,19 +5148,19 @@
         <v>9</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>282</v>
+        <v>263</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>373</v>
+        <v>353</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>439</v>
+        <v>419</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>283</v>
+        <v>264</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>284</v>
+        <v>265</v>
       </c>
       <c r="I90" s="1">
         <v>55.34</v>
@@ -5180,31 +5174,31 @@
       <c r="L90" s="3">
         <v>40796</v>
       </c>
-      <c r="M90" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="91" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M90" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>285</v>
+        <v>266</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>329</v>
+        <v>309</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>353</v>
+        <v>333</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>439</v>
+        <v>419</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>287</v>
+        <v>268</v>
       </c>
       <c r="I91" s="1">
         <v>37.36</v>
@@ -5218,11 +5212,11 @@
       <c r="L91" s="3">
         <v>44197</v>
       </c>
-      <c r="M91" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="92" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M91" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>146</v>
       </c>
@@ -5230,19 +5224,19 @@
         <v>9</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>288</v>
+        <v>269</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>382</v>
+        <v>362</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>434</v>
+        <v>414</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>290</v>
+        <v>271</v>
       </c>
       <c r="I92" s="1">
         <v>46.58</v>
@@ -5256,11 +5250,11 @@
       <c r="L92" s="3">
         <v>40796</v>
       </c>
-      <c r="M92" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="93" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M92" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>147</v>
       </c>
@@ -5268,19 +5262,19 @@
         <v>9</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>291</v>
+        <v>272</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>373</v>
+        <v>353</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>440</v>
+        <v>420</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>292</v>
+        <v>273</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>293</v>
+        <v>274</v>
       </c>
       <c r="I93" s="1">
         <v>68.38</v>
@@ -5294,11 +5288,11 @@
       <c r="L93" s="3">
         <v>40796</v>
       </c>
-      <c r="M93" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M93" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>151</v>
       </c>
@@ -5306,19 +5300,19 @@
         <v>9</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>294</v>
+        <v>275</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>339</v>
+        <v>319</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>441</v>
+        <v>421</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>295</v>
+        <v>276</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>296</v>
+        <v>277</v>
       </c>
       <c r="I94" s="1">
         <v>36.950000000000003</v>
@@ -5332,31 +5326,31 @@
       <c r="L94" s="3">
         <v>40796</v>
       </c>
-      <c r="M94" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="95" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M94" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>297</v>
+        <v>278</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>298</v>
+        <v>279</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>383</v>
+        <v>363</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>441</v>
+        <v>421</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>299</v>
+        <v>280</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>300</v>
+        <v>281</v>
       </c>
       <c r="I95" s="1">
         <v>26.55</v>
@@ -5370,11 +5364,11 @@
       <c r="L95" s="3">
         <v>44197</v>
       </c>
-      <c r="M95" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="96" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M95" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>156</v>
       </c>
@@ -5382,22 +5376,22 @@
         <v>9</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>301</v>
+        <v>282</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>355</v>
+        <v>335</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>442</v>
+        <v>422</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>302</v>
+        <v>283</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="I96" s="1" t="s">
-        <v>304</v>
+        <v>284</v>
+      </c>
+      <c r="I96" s="1">
+        <v>44.75</v>
       </c>
       <c r="J96" s="1" t="s">
         <v>9</v>
@@ -5408,11 +5402,11 @@
       <c r="L96" s="3">
         <v>40796</v>
       </c>
-      <c r="M96" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="97" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M96" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>28</v>
       </c>
@@ -5420,19 +5414,19 @@
         <v>9</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>330</v>
+        <v>310</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>365</v>
+        <v>345</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>443</v>
+        <v>423</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>305</v>
+        <v>285</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
       <c r="I97" s="1">
         <v>23.45</v>
@@ -5446,11 +5440,11 @@
       <c r="L97" s="3">
         <v>44409</v>
       </c>
-      <c r="M97" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="98" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M97" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>3</v>
       </c>
@@ -5458,19 +5452,19 @@
         <v>9</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>307</v>
+        <v>287</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>339</v>
+        <v>319</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>444</v>
+        <v>424</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>308</v>
+        <v>288</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>309</v>
+        <v>289</v>
       </c>
       <c r="I98" s="1">
         <v>18.28</v>
@@ -5484,11 +5478,12 @@
       <c r="L98" s="3">
         <v>44805</v>
       </c>
-      <c r="M98" s="1" t="s">
-        <v>10</v>
+      <c r="M98" s="2" t="s">
+        <v>429</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>